<commit_message>
v 2.0 learning to set weights on your own and not take into account outliers from the sample
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrejusycenko/PycharmProjects/bino/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79FC167-58C5-AC46-BDD1-0FF21B35E4AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5927DC8E-DEE7-2045-AE02-4F1513202A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17300" xr2:uid="{4571DB51-E391-6843-8868-81228BAA0884}"/>
   </bookViews>
@@ -408,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB659BE-57D3-4B4F-8ABC-6EE083E0D0D9}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>